<commit_message>
updated listeners, basic tests
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/DataSheet.xlsx
+++ b/src/test/resources/testData/DataSheet.xlsx
@@ -1,13 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20374"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A90634A-EC65-45E8-8774-57BC9DE204F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DATA" sheetId="1" r:id="rId1"/>
+    <sheet name="RunManager" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,37 +21,79 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>fname</t>
-  </si>
-  <si>
-    <t>lname</t>
-  </si>
-  <si>
-    <t>Matt</t>
-  </si>
-  <si>
-    <t>Damon</t>
-  </si>
-  <si>
-    <t>Homer</t>
-  </si>
-  <si>
-    <t>Simpson</t>
-  </si>
-  <si>
-    <t>Wayne</t>
-  </si>
-  <si>
-    <t>Bruce</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
+  <si>
+    <t>TestName</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>execute</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>loginTestUsingValidData</t>
+  </si>
+  <si>
+    <t>loginTestUsingBlankEmail</t>
+  </si>
+  <si>
+    <t>loginTestUsingInvalidPassword</t>
+  </si>
+  <si>
+    <t>To perform login to application using valid email and password</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>To perform login to application using valid email and invalid password</t>
+  </si>
+  <si>
+    <t>To perform login to application using blank email and valid password</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>admin@yourstore.com</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>ad</t>
+  </si>
+  <si>
+    <t>admi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -57,16 +101,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -74,12 +132,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -109,7 +192,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -387,48 +470,181 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F9CD85D-55A1-42DA-8F51-30584EA1A32F}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>